<commit_message>
Uploaded gene trees for all core Megalocytivirus core genes.
G0000000 have been annotated. The other core gene trees have not.
</commit_message>
<xml_diff>
--- a/20240807_Genetic information spreadsheet_megalocytiviruses.xlsx
+++ b/20240807_Genetic information spreadsheet_megalocytiviruses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://csiroau-my.sharepoint.com/personal/han394_csiro_au/Documents/Documents/GitHub/Phylogenomic-study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="123" documentId="8_{BBE3224F-4570-4915-A6DB-5FBC4F9097C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2B2ED2F2-1204-4398-B829-1D209367E784}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="8_{BBE3224F-4570-4915-A6DB-5FBC4F9097C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{7E6799DA-BCB5-48D5-8825-4B7067C6CD8D}"/>
   <bookViews>
-    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="13656" xr2:uid="{CD6C468C-256F-45C2-B81B-3E7578C677C5}"/>
+    <workbookView minimized="1" xWindow="2712" yWindow="1236" windowWidth="15684" windowHeight="13440" xr2:uid="{CD6C468C-256F-45C2-B81B-3E7578C677C5}"/>
   </bookViews>
   <sheets>
     <sheet name="Main sheet" sheetId="1" r:id="rId1"/>
@@ -41691,9 +41691,9 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:Y547"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="50" zoomScaleNormal="50" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E13" sqref="E13"/>
+      <selection pane="topRight" activeCell="Q99" sqref="Q99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -42590,7 +42590,7 @@
         <v>1725</v>
       </c>
     </row>
-    <row r="13" spans="1:24" ht="216" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" ht="216" hidden="1" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>801</v>
       </c>
@@ -66468,7 +66468,7 @@
         <v>1296</v>
       </c>
     </row>
-    <row r="376" spans="1:24" ht="187.2" hidden="1" x14ac:dyDescent="0.3">
+    <row r="376" spans="1:24" ht="187.2" x14ac:dyDescent="0.3">
       <c r="A376" s="10" t="s">
         <v>1349</v>
       </c>
@@ -74279,7 +74279,7 @@
   <autoFilter ref="A1:X490" xr:uid="{F8DAEBFD-78AC-4E24-A1EF-CD140122AED7}">
     <filterColumn colId="0">
       <filters>
-        <filter val="KC244182"/>
+        <filter val="_x0009__x000a_NC_005946"/>
       </filters>
     </filterColumn>
   </autoFilter>

</xml_diff>